<commit_message>
Adapt SerDe serializing. * Add Nullable annotation and defaul value for undefined json properties.
</commit_message>
<xml_diff>
--- a/blanco-meta/telegrams/ApiTelegram.xlsx
+++ b/blanco-meta/telegrams/ApiTelegram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/nanosys/SumidaMeta/meta/common/telegrams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-api-core/blanco-meta/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C108390-153C-F243-AF96-85AC12D0C9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6869F35-550A-8E4A-A31D-661C54F5723F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="5060" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="5040" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -51,10 +51,21 @@
     <definedName name="必須" localSheetId="1">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="4"/>
@@ -64,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>クラス名</t>
   </si>
@@ -452,6 +463,35 @@
   </si>
   <si>
     <t>%%</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>kotlinでは無視</t>
+    <rPh sb="0" eb="4">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">ヘンスウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Nullable</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>必須</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヒッス </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@Nullable</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>io.micronaut.core.annotation.Nullable</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1080,26 +1120,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1111,25 +1150,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1168,14 +1206,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1197,7 +1230,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1214,9 +1246,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1225,11 +1255,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1238,7 +1268,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1655,10 +1685,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1669,11 +1699,12 @@
     <col min="6" max="6" width="6.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" style="1" customWidth="1"/>
-    <col min="9" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="34.33203125" style="1" customWidth="1"/>
+    <col min="10" max="15" width="14" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19">
+    <row r="1" spans="1:15" ht="19">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1681,17 +1712,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:15">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:15">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1699,7 +1730,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1710,7 +1741,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1721,7 +1752,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1732,53 +1763,53 @@
       <c r="D8" s="11"/>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:12" s="34" customFormat="1">
-      <c r="A9" s="51" t="s">
+    <row r="9" spans="1:15">
+      <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="34" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="34" customFormat="1">
-      <c r="A10" s="85" t="s">
+    <row r="10" spans="1:15">
+      <c r="A10" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="73" t="s">
+      <c r="B10" s="76"/>
+      <c r="C10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="74"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="34" t="s">
+      <c r="D10" s="65"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="34" customFormat="1">
-      <c r="A11" s="51" t="s">
+    <row r="11" spans="1:15">
+      <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="75"/>
-    </row>
-    <row r="12" spans="1:12" s="34" customFormat="1">
-      <c r="A12" s="51" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="79" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="D12" s="65"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1791,7 +1822,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -1804,12 +1835,12 @@
       <c r="F14" s="12"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:12" s="34" customFormat="1">
-      <c r="A15" s="48" t="s">
+    <row r="15" spans="1:15">
+      <c r="A15" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="47" t="s">
         <v>49</v>
       </c>
       <c r="D15"/>
@@ -1821,13 +1852,16 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
-    </row>
-    <row r="16" spans="1:12" s="34" customFormat="1">
-      <c r="A16" s="48" t="s">
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="50"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="47"/>
       <c r="D16" t="s">
         <v>50</v>
       </c>
@@ -1839,13 +1873,16 @@
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" s="34" customFormat="1">
-      <c r="A17" s="48" t="s">
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="50"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="47"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
@@ -1855,13 +1892,16 @@
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" s="34" customFormat="1">
-      <c r="A18" s="48" t="s">
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="47"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -1871,24 +1911,27 @@
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" s="34" customFormat="1">
-      <c r="A19" s="48" t="s">
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="47"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:12" s="34" customFormat="1">
-      <c r="A20" s="48" t="s">
+    <row r="20" spans="1:15">
+      <c r="A20" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="47" t="s">
         <v>30</v>
       </c>
       <c r="D20"/>
@@ -1896,23 +1939,23 @@
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:12" s="34" customFormat="1">
-      <c r="A21" s="48" t="s">
+    <row r="21" spans="1:15">
+      <c r="A21" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="50"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="47"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:12" s="34" customFormat="1">
-      <c r="A22" s="71" t="s">
+    <row r="22" spans="1:15">
+      <c r="A22" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="50" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="47" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
@@ -1925,13 +1968,16 @@
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12" s="34" customFormat="1">
-      <c r="A23" s="71" t="s">
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="50" t="s">
+      <c r="B23" s="64"/>
+      <c r="C23" s="47" t="s">
         <v>30</v>
       </c>
       <c r="D23" t="s">
@@ -1944,56 +1990,59 @@
       <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:12" s="34" customFormat="1">
-      <c r="A25" s="31" t="s">
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-    </row>
-    <row r="26" spans="1:12" s="34" customFormat="1">
-      <c r="A26" s="35" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-    </row>
-    <row r="27" spans="1:12" s="34" customFormat="1">
-      <c r="A27" s="51" t="s">
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="38"/>
-    </row>
-    <row r="28" spans="1:12" s="34" customFormat="1">
-      <c r="A28" s="51" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="36"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="38"/>
-    </row>
-    <row r="29" spans="1:12" s="34" customFormat="1">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="36"/>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -2002,77 +2051,97 @@
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:12" s="34" customFormat="1">
-      <c r="A30" s="31" t="s">
+    <row r="30" spans="1:15">
+      <c r="A30" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="55"/>
-    </row>
-    <row r="31" spans="1:12" s="34" customFormat="1">
-      <c r="A31" s="56" t="s">
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="48"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="58"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-    </row>
-    <row r="32" spans="1:12" s="34" customFormat="1">
-      <c r="A32" s="60">
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="51"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="52"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="53">
         <v>1</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="64"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="9"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
-    </row>
-    <row r="33" spans="1:11" s="34" customFormat="1">
-      <c r="A33" s="60"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="64"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="53">
+        <v>2</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="9"/>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
-    </row>
-    <row r="34" spans="1:11" s="34" customFormat="1">
-      <c r="A34" s="67"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="64"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="9"/>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
-    </row>
-    <row r="35" spans="1:11" s="34" customFormat="1">
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -2082,297 +2151,385 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:15">
       <c r="A36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
       <c r="H36" s="6"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="80"/>
-    </row>
-    <row r="37" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A37" s="88" t="s">
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="70"/>
+      <c r="N36" s="70"/>
+      <c r="O36" s="70"/>
+    </row>
+    <row r="37" spans="1:15" ht="13.5" customHeight="1">
+      <c r="A37" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="88" t="s">
+      <c r="B37" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="87" t="s">
+      <c r="C37" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="87" t="s">
+      <c r="D37" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="87" t="s">
+      <c r="E37" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="87"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="84" t="s">
+      <c r="F37" s="77"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="J37" s="84" t="s">
+      <c r="K37" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="L37" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="K37" s="84" t="s">
+      <c r="N37" s="74" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="88"/>
-      <c r="B38" s="88"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="84"/>
-      <c r="J38" s="84"/>
-      <c r="K38" s="84"/>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="18">
+      <c r="O37" s="74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="78"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="74"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="74"/>
+      <c r="O38" s="74"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="17">
         <v>1</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="81" t="s">
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="18">
+      <c r="K39" s="71"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="71"/>
+      <c r="N39" s="71"/>
+      <c r="O39" s="71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="17">
         <v>2</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="81" t="s">
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="J40" s="81" t="s">
+      <c r="K40" s="71"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="K40" s="81" t="s">
+      <c r="N40" s="71" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="81"/>
-      <c r="J41" s="81"/>
-      <c r="K41" s="81"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="81"/>
-      <c r="J42" s="81"/>
-      <c r="K42" s="81"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="82"/>
-      <c r="K43" s="82"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="18"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="81"/>
-      <c r="J44" s="81"/>
-      <c r="K44" s="81"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="82"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="81"/>
-      <c r="J46" s="81"/>
-      <c r="K46" s="81"/>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="18"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="81"/>
-      <c r="J48" s="81"/>
-      <c r="K48" s="81"/>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="18"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="81"/>
-      <c r="J49" s="81"/>
-      <c r="K49" s="81"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="81"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="81"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="81"/>
-      <c r="J51" s="81"/>
-      <c r="K51" s="81"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="18"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="81"/>
-      <c r="J52" s="81"/>
-      <c r="K52" s="81"/>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="23"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="83"/>
-      <c r="J53" s="83"/>
-      <c r="K53" s="83"/>
+      <c r="O40" s="71"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
+      <c r="N41" s="71"/>
+      <c r="O41" s="71"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="17"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="71"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="71"/>
+      <c r="O42" s="71"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="17"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="72"/>
+      <c r="O43" s="72"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="17"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="71"/>
+      <c r="J44" s="71"/>
+      <c r="K44" s="71"/>
+      <c r="L44" s="71"/>
+      <c r="M44" s="71"/>
+      <c r="N44" s="71"/>
+      <c r="O44" s="71"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="72"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="72"/>
+      <c r="M45" s="72"/>
+      <c r="N45" s="72"/>
+      <c r="O45" s="72"/>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="71"/>
+      <c r="J46" s="71"/>
+      <c r="K46" s="71"/>
+      <c r="L46" s="71"/>
+      <c r="M46" s="71"/>
+      <c r="N46" s="71"/>
+      <c r="O46" s="71"/>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="17"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="72"/>
+      <c r="J47" s="72"/>
+      <c r="K47" s="72"/>
+      <c r="L47" s="72"/>
+      <c r="M47" s="72"/>
+      <c r="N47" s="72"/>
+      <c r="O47" s="72"/>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="17"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="71"/>
+      <c r="J48" s="71"/>
+      <c r="K48" s="71"/>
+      <c r="L48" s="71"/>
+      <c r="M48" s="71"/>
+      <c r="N48" s="71"/>
+      <c r="O48" s="71"/>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="17"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="71"/>
+      <c r="K49" s="71"/>
+      <c r="L49" s="71"/>
+      <c r="M49" s="71"/>
+      <c r="N49" s="71"/>
+      <c r="O49" s="71"/>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="17"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="71"/>
+      <c r="J50" s="71"/>
+      <c r="K50" s="71"/>
+      <c r="L50" s="71"/>
+      <c r="M50" s="71"/>
+      <c r="N50" s="71"/>
+      <c r="O50" s="71"/>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="17"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="71"/>
+      <c r="K51" s="71"/>
+      <c r="L51" s="71"/>
+      <c r="M51" s="71"/>
+      <c r="N51" s="71"/>
+      <c r="O51" s="71"/>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="17"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="71"/>
+      <c r="J52" s="71"/>
+      <c r="K52" s="71"/>
+      <c r="L52" s="71"/>
+      <c r="M52" s="71"/>
+      <c r="N52" s="71"/>
+      <c r="O52" s="71"/>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" s="22"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="73"/>
+      <c r="J53" s="73"/>
+      <c r="K53" s="73"/>
+      <c r="L53" s="73"/>
+      <c r="M53" s="73"/>
+      <c r="N53" s="73"/>
+      <c r="O53" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="O37:O38"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="N37:N38"/>
     <mergeCell ref="J37:J38"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="I37:I38"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="E37:F38"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D37:D38"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="I37:I38"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="8">
@@ -2423,107 +2580,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="41" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="41" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="41" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="41" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="41" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="41" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="41" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="15" max="261" width="8.83203125" style="41" customWidth="1"/>
-    <col min="262" max="16384" width="10.83203125" style="41"/>
+    <col min="1" max="3" width="8.83203125" style="39" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="39" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="39" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="39" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="39" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="261" width="8.83203125" style="39" customWidth="1"/>
+    <col min="262" max="16384" width="10.83203125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="19">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="40"/>
+      <c r="R1" s="38"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="42" t="s">
+      <c r="P3" s="40" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="B4" s="43"/>
-      <c r="D4" s="76" t="s">
+      <c r="B4" s="41"/>
+      <c r="D4" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="P4" s="44"/>
+      <c r="H4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="P4" s="42"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="F5" s="46"/>
-      <c r="H5" s="46" t="s">
+      <c r="D5" s="67"/>
+      <c r="F5" s="44"/>
+      <c r="H5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="46" t="s">
+      <c r="L5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="N5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="46" t="s">
+      <c r="P5" s="44" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="47"/>
+      <c r="B6" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>

<commit_message>
Auto add @Nullable to non-required properties.
</commit_message>
<xml_diff>
--- a/blanco-meta/telegrams/ApiTelegram.xlsx
+++ b/blanco-meta/telegrams/ApiTelegram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-api-core/blanco-meta/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6869F35-550A-8E4A-A31D-661C54F5723F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2E8B5F-C4BA-894A-B591-C77FFAE5864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7380" yWindow="5040" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>クラス名</t>
   </si>
@@ -484,10 +484,6 @@
     <rPh sb="0" eb="2">
       <t xml:space="preserve">ヒッス </t>
     </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>@Nullable</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -1687,8 +1683,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2108,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="57"/>
@@ -2278,9 +2274,7 @@
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="21"/>
-      <c r="I40" s="72" t="s">
-        <v>70</v>
-      </c>
+      <c r="I40" s="72"/>
       <c r="J40" s="71" t="s">
         <v>30</v>
       </c>

</xml_diff>